<commit_message>
"Complete system: Add flexible assignment option + dual-mode main script
- Implement flexible_pmp_assignment.py for all-PMP assignment (3+ PMPs per project)
- Update run_complete_analysis.py with --flexible flag support
- Both modes: standard (2 PMPs/charity) and flexible (all PMPs assigned)
- Update documentation (README.md, SETUP.md) for dual assignment modes
- Test both modes successfully: 20 PMPs (standard) vs 22 PMPs (flexible)
- Capacity-based assignment in flexible mode for optimal resource utilization"
</commit_message>
<xml_diff>
--- a/LinkedIn_Analysis_Report.xlsx
+++ b/LinkedIn_Analysis_Report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,12 @@
     <t>Ryan Benedek</t>
   </si>
   <si>
+    <t>Jacqueline Shen</t>
+  </si>
+  <si>
+    <t>Nikki Gittins</t>
+  </si>
+  <si>
     <t>linkedin.com/in/mariamainhardt</t>
   </si>
   <si>
@@ -153,6 +159,9 @@
     <t>https://www.linkedin.com/in/ryan-benedek/</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/jacqueline-shen-5b565917a/</t>
+  </si>
+  <si>
     <t>https://linkedin.com/in/mariamainhardt</t>
   </si>
   <si>
@@ -237,13 +246,13 @@
     <t>Avg Profile Completeness</t>
   </si>
   <si>
-    <t>85.0%</t>
-  </si>
-  <si>
-    <t>7.6</t>
-  </si>
-  <si>
-    <t>9.4</t>
+    <t>81.8%</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>9.3</t>
   </si>
 </sst>
 </file>
@@ -614,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -645,19 +654,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -665,19 +674,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -685,19 +694,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E4">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -705,19 +714,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -725,19 +734,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -745,19 +754,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -765,19 +774,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -785,7 +794,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -794,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -802,19 +811,19 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -822,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -831,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -839,19 +848,19 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -859,7 +868,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -868,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -876,19 +885,19 @@
         <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E14">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -896,19 +905,19 @@
         <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -916,19 +925,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E16">
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -936,19 +945,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E17">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -956,19 +965,19 @@
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -976,19 +985,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E19">
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -996,19 +1005,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E20">
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1016,19 +1025,56 @@
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1059,6 +1105,8 @@
     <hyperlink ref="D20" r:id="rId24"/>
     <hyperlink ref="B21" r:id="rId25"/>
     <hyperlink ref="D21" r:id="rId26"/>
+    <hyperlink ref="B22" r:id="rId27"/>
+    <hyperlink ref="D22" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1066,7 +1114,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1074,25 +1122,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1100,7 +1148,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -1112,10 +1160,10 @@
         <v>3.61</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1123,7 +1171,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1135,10 +1183,10 @@
         <v>4.91</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1146,7 +1194,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -1158,10 +1206,10 @@
         <v>2.2</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1169,7 +1217,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -1181,10 +1229,10 @@
         <v>3.83</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1192,7 +1240,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -1204,10 +1252,10 @@
         <v>4.53</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1215,7 +1263,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -1227,10 +1275,10 @@
         <v>5.99</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1238,7 +1286,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -1250,10 +1298,10 @@
         <v>5.07</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1270,10 +1318,10 @@
         <v>4.71</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1281,7 +1329,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1293,10 +1341,10 @@
         <v>3.96</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1313,10 +1361,10 @@
         <v>4.32</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1324,7 +1372,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -1336,10 +1384,10 @@
         <v>5.19</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1347,7 +1395,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1359,10 +1407,10 @@
         <v>3.5</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1370,7 +1418,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>8</v>
@@ -1382,10 +1430,10 @@
         <v>3.15</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1393,7 +1441,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -1405,10 +1453,10 @@
         <v>4.73</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1416,7 +1464,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -1428,10 +1476,10 @@
         <v>3.84</v>
       </c>
       <c r="F16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1439,7 +1487,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -1451,10 +1499,10 @@
         <v>5.56</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1462,7 +1510,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -1474,10 +1522,10 @@
         <v>5.68</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1485,7 +1533,7 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>8</v>
@@ -1497,10 +1545,10 @@
         <v>4.68</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1508,7 +1556,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -1520,10 +1568,10 @@
         <v>3.1</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1531,7 +1579,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1543,10 +1591,53 @@
         <v>4.5</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>4.37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>4.94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1560,6 +1651,7 @@
     <hyperlink ref="B15" r:id="rId7"/>
     <hyperlink ref="B18" r:id="rId8"/>
     <hyperlink ref="B21" r:id="rId9"/>
+    <hyperlink ref="B22" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1575,50 +1667,50 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add dynamic file detection for automatic latest file selection
- Created dynamic_file_loader.py for automatic file detection
- Modified run_complete_analysis.py to use dynamic file selection
- Updated enhanced_pmp_charity_matching.py to support dynamic file paths
- Updated generate_email_drafts.py to use latest files automatically
- System now automatically finds and uses most recently modified registration files
- No longer requires exact filename matches - works with any naming convention
- Added latest registration data file (25092025) with 33 PMPs vs previous 29
- Generated updated analysis reports with new data
</commit_message>
<xml_diff>
--- a/LinkedIn_Analysis_Report.xlsx
+++ b/LinkedIn_Analysis_Report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -102,6 +102,39 @@
     <t>Nikki Gittins</t>
   </si>
   <si>
+    <t>Peter Harrison</t>
+  </si>
+  <si>
+    <t>Aishwarya  Rajendran</t>
+  </si>
+  <si>
+    <t>Carolina Abelha Melo</t>
+  </si>
+  <si>
+    <t>Ivonne Portocarrero</t>
+  </si>
+  <si>
+    <t>Richard John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sameh  Megally </t>
+  </si>
+  <si>
+    <t>Achintya Hrishikesh</t>
+  </si>
+  <si>
+    <t>Julia Wright</t>
+  </si>
+  <si>
+    <t>Emma  Voss</t>
+  </si>
+  <si>
+    <t>Lindsey Norris</t>
+  </si>
+  <si>
+    <t>Hadi Ahmadi</t>
+  </si>
+  <si>
     <t>linkedin.com/in/mariamainhardt</t>
   </si>
   <si>
@@ -162,6 +195,24 @@
     <t>https://www.linkedin.com/in/jacqueline-shen-5b565917a/</t>
   </si>
   <si>
+    <t>linkedin.com/in/aishwarya-rajendran2012</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sameh-megally-8aa66a7b?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/achintya-h-10b694227/</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/juliawright1</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/emma-voss-07a91341</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hadiahmadipmp/</t>
+  </si>
+  <si>
     <t>https://linkedin.com/in/mariamainhardt</t>
   </si>
   <si>
@@ -186,6 +237,15 @@
     <t>https://www.linkedin.com/in/shreya-shah-s</t>
   </si>
   <si>
+    <t>https://linkedin.com/in/aishwarya-rajendran2012</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/juliawright1</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/emma-voss-07a91341</t>
+  </si>
+  <si>
     <t>[]</t>
   </si>
   <si>
@@ -246,13 +306,13 @@
     <t>Avg Profile Completeness</t>
   </si>
   <si>
-    <t>81.8%</t>
-  </si>
-  <si>
-    <t>7.4</t>
-  </si>
-  <si>
-    <t>9.3</t>
+    <t>72.7%</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>9.2</t>
   </si>
 </sst>
 </file>
@@ -623,7 +683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -654,19 +714,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="E2">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -674,19 +734,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -694,19 +754,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="E4">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -714,19 +774,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -734,19 +794,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -754,19 +814,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -774,19 +834,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E8">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -794,7 +854,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -803,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -811,19 +871,19 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -831,7 +891,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -840,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -848,19 +908,19 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -868,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -877,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -885,19 +945,19 @@
         <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -905,19 +965,19 @@
         <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -925,19 +985,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="E16">
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -945,19 +1005,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="E17">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -965,19 +1025,19 @@
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -985,19 +1045,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E19">
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1005,19 +1065,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E20">
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1025,19 +1085,19 @@
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1045,19 +1105,19 @@
         <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1065,16 +1125,221 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>57</v>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1107,6 +1372,15 @@
     <hyperlink ref="D21" r:id="rId26"/>
     <hyperlink ref="B22" r:id="rId27"/>
     <hyperlink ref="D22" r:id="rId28"/>
+    <hyperlink ref="D25" r:id="rId29"/>
+    <hyperlink ref="B29" r:id="rId30"/>
+    <hyperlink ref="D29" r:id="rId31"/>
+    <hyperlink ref="B30" r:id="rId32"/>
+    <hyperlink ref="D30" r:id="rId33"/>
+    <hyperlink ref="D31" r:id="rId34"/>
+    <hyperlink ref="D32" r:id="rId35"/>
+    <hyperlink ref="B34" r:id="rId36"/>
+    <hyperlink ref="D34" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1114,7 +1388,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,25 +1396,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1148,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -1160,10 +1434,10 @@
         <v>3.61</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1171,7 +1445,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1183,10 +1457,10 @@
         <v>4.91</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1194,7 +1468,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -1206,10 +1480,10 @@
         <v>2.2</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1217,7 +1491,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -1229,10 +1503,10 @@
         <v>3.83</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1240,7 +1514,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -1252,10 +1526,10 @@
         <v>4.53</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1263,7 +1537,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -1275,10 +1549,10 @@
         <v>5.99</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1286,7 +1560,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -1298,10 +1572,10 @@
         <v>5.07</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1318,10 +1592,10 @@
         <v>4.71</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1329,7 +1603,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1341,10 +1615,10 @@
         <v>3.96</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1361,10 +1635,10 @@
         <v>4.32</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1372,7 +1646,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -1384,10 +1658,10 @@
         <v>5.19</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1395,7 +1669,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1407,10 +1681,10 @@
         <v>3.5</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1418,7 +1692,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>8</v>
@@ -1430,10 +1704,10 @@
         <v>3.15</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1441,7 +1715,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -1453,10 +1727,10 @@
         <v>4.73</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1464,7 +1738,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -1476,10 +1750,10 @@
         <v>3.84</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1487,7 +1761,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -1499,10 +1773,10 @@
         <v>5.56</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1510,7 +1784,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -1522,10 +1796,10 @@
         <v>5.68</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1533,7 +1807,7 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <v>8</v>
@@ -1545,10 +1819,10 @@
         <v>4.68</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1556,7 +1830,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -1568,10 +1842,10 @@
         <v>3.1</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1579,7 +1853,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1591,10 +1865,10 @@
         <v>4.5</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1602,7 +1876,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1614,10 +1888,10 @@
         <v>4.37</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1634,10 +1908,248 @@
         <v>4.94</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>3.99</v>
+      </c>
+      <c r="F24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>2.48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>3.37</v>
+      </c>
+      <c r="F26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>2.86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>3.94</v>
+      </c>
+      <c r="F28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>5.04</v>
+      </c>
+      <c r="F29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>4.45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>4.84</v>
+      </c>
+      <c r="F31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <v>6.25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>4.71</v>
+      </c>
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>5.81</v>
+      </c>
+      <c r="F34" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1652,6 +2164,9 @@
     <hyperlink ref="B18" r:id="rId8"/>
     <hyperlink ref="B21" r:id="rId9"/>
     <hyperlink ref="B22" r:id="rId10"/>
+    <hyperlink ref="B29" r:id="rId11"/>
+    <hyperlink ref="B30" r:id="rId12"/>
+    <hyperlink ref="B34" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1667,50 +2182,50 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>